<commit_message>
Update design and document
</commit_message>
<xml_diff>
--- a/design/KhaiQuatManHinh.xlsx
+++ b/design/KhaiQuatManHinh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\watch-store\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0AEA31-2A3C-41C8-AD94-39A312166D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B610CACA-8995-4A2A-9E1B-AD7EA952B13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="799" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="799" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Header" sheetId="1" r:id="rId1"/>
@@ -208,22 +208,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -9458,6 +9445,189 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D205159-AF11-BD8E-D080-3E86E36CC3D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2552700" y="1270000"/>
+          <a:ext cx="3467100" cy="2012950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAB3EC21-A530-427E-82F1-7532C032075A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2565400" y="3390900"/>
+          <a:ext cx="3467100" cy="1327150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Callout: Left Arrow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA6319AF-DC09-B49A-5C4B-F427544E30EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6083300" y="1689100"/>
+          <a:ext cx="736600" cy="527050"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrowCallout">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&lt;a&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9878,6 +10048,258 @@
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> ký</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Callout: Right Arrow 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE0D4DE0-B903-920B-8ECC-12E26EAB4262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="939800" y="2228850"/>
+          <a:ext cx="1308100" cy="742950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrowCallout">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&lt;input</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> type="submit"</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Callout: Left Arrow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66FFCF9D-819C-5073-6310-95413E715608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4394200" y="1828800"/>
+          <a:ext cx="1250950" cy="787400"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrowCallout">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&lt;input type="password"&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Callout: Down Arrow 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE98236B-576F-B788-0882-07E1B5130B22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3556000" y="584200"/>
+          <a:ext cx="1092200" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrowCallout">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>&lt;input type="email"&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rectangle 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11846E33-EF89-E612-556C-45FA61D6FF07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3651250" y="2825750"/>
+          <a:ext cx="558800" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -10215,449 +10637,449 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="23" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="8"/>
-      <c r="AC23" s="8"/>
-      <c r="AD23" s="8"/>
-      <c r="AE23" s="8"/>
-      <c r="AF23" s="8"/>
-      <c r="AG23" s="8"/>
-      <c r="AH23" s="8"/>
-      <c r="AI23" s="8"/>
-      <c r="AJ23" s="8"/>
-      <c r="AK23" s="8"/>
-      <c r="AL23" s="8"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
+      <c r="AG23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
     </row>
     <row r="24" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B24" s="8"/>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="8"/>
-      <c r="AA24" s="8"/>
-      <c r="AB24" s="8"/>
-      <c r="AC24" s="8"/>
-      <c r="AD24" s="8"/>
-      <c r="AE24" s="8"/>
-      <c r="AF24" s="8"/>
-      <c r="AG24" s="8"/>
-      <c r="AH24" s="8"/>
-      <c r="AI24" s="8"/>
-      <c r="AJ24" s="8"/>
-      <c r="AK24" s="8"/>
-      <c r="AL24" s="8"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
     </row>
     <row r="25" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B25" s="8"/>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="8"/>
-      <c r="AA25" s="8"/>
-      <c r="AB25" s="8"/>
-      <c r="AC25" s="8"/>
-      <c r="AD25" s="8"/>
-      <c r="AE25" s="8"/>
-      <c r="AF25" s="8"/>
-      <c r="AG25" s="8"/>
-      <c r="AH25" s="8"/>
-      <c r="AI25" s="8"/>
-      <c r="AJ25" s="8"/>
-      <c r="AK25" s="8"/>
-      <c r="AL25" s="8"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
+      <c r="AG25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
     </row>
     <row r="26" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="11" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
-      <c r="V26" s="8"/>
-      <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="8"/>
-      <c r="AA26" s="8"/>
-      <c r="AB26" s="8"/>
-      <c r="AC26" s="8"/>
-      <c r="AD26" s="8"/>
-      <c r="AE26" s="8"/>
-      <c r="AF26" s="8"/>
-      <c r="AG26" s="8"/>
-      <c r="AH26" s="8"/>
-      <c r="AI26" s="8"/>
-      <c r="AJ26" s="8"/>
-      <c r="AK26" s="8"/>
-      <c r="AL26" s="8"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
     </row>
     <row r="27" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="11" t="s">
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="Q27" s="8"/>
-      <c r="R27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="T27" s="8"/>
-      <c r="U27" s="8"/>
-      <c r="V27" s="8"/>
-      <c r="W27" s="8"/>
-      <c r="X27" s="8"/>
-      <c r="Y27" s="8"/>
-      <c r="Z27" s="8"/>
-      <c r="AA27" s="8"/>
-      <c r="AB27" s="8"/>
-      <c r="AC27" s="8"/>
-      <c r="AD27" s="8"/>
-      <c r="AE27" s="8"/>
-      <c r="AF27" s="8"/>
-      <c r="AG27" s="8"/>
-      <c r="AH27" s="8"/>
-      <c r="AI27" s="8"/>
-      <c r="AJ27" s="8"/>
-      <c r="AK27" s="8"/>
-      <c r="AL27" s="8"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
     </row>
     <row r="28" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-      <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="T28" s="8"/>
-      <c r="U28" s="8"/>
-      <c r="V28" s="8"/>
-      <c r="W28" s="8"/>
-      <c r="X28" s="8"/>
-      <c r="Y28" s="8"/>
-      <c r="Z28" s="8"/>
-      <c r="AA28" s="8"/>
-      <c r="AB28" s="8"/>
-      <c r="AC28" s="8"/>
-      <c r="AD28" s="8"/>
-      <c r="AE28" s="8"/>
-      <c r="AF28" s="8"/>
-      <c r="AG28" s="8"/>
-      <c r="AH28" s="8"/>
-      <c r="AI28" s="8"/>
-      <c r="AJ28" s="8"/>
-      <c r="AK28" s="8"/>
-      <c r="AL28" s="8"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="U28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
     </row>
     <row r="29" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B29" s="8"/>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-      <c r="R29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="T29" s="8"/>
-      <c r="U29" s="8"/>
-      <c r="V29" s="8"/>
-      <c r="W29" s="8"/>
-      <c r="X29" s="8"/>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-      <c r="AB29" s="8"/>
-      <c r="AC29" s="8"/>
-      <c r="AD29" s="8"/>
-      <c r="AE29" s="8"/>
-      <c r="AF29" s="8"/>
-      <c r="AG29" s="8"/>
-      <c r="AH29" s="8"/>
-      <c r="AI29" s="8"/>
-      <c r="AJ29" s="8"/>
-      <c r="AK29" s="8"/>
-      <c r="AL29" s="8"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="U29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Y29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
+      <c r="AG29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
     </row>
     <row r="30" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="11" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="8"/>
-      <c r="Q30" s="8"/>
-      <c r="R30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="T30" s="8"/>
-      <c r="U30" s="8"/>
-      <c r="V30" s="8"/>
-      <c r="W30" s="8"/>
-      <c r="X30" s="8"/>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="8"/>
-      <c r="AC30" s="8"/>
-      <c r="AD30" s="8"/>
-      <c r="AE30" s="8"/>
-      <c r="AF30" s="8"/>
-      <c r="AG30" s="8"/>
-      <c r="AH30" s="8"/>
-      <c r="AI30" s="8"/>
-      <c r="AJ30" s="8"/>
-      <c r="AK30" s="8"/>
-      <c r="AL30" s="8"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="U30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
     </row>
     <row r="31" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="11" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="8"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="8"/>
-      <c r="Q31" s="8"/>
-      <c r="R31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="T31" s="8"/>
-      <c r="U31" s="8"/>
-      <c r="V31" s="8"/>
-      <c r="W31" s="8"/>
-      <c r="X31" s="8"/>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
-      <c r="AB31" s="8"/>
-      <c r="AC31" s="8"/>
-      <c r="AD31" s="8"/>
-      <c r="AE31" s="8"/>
-      <c r="AF31" s="8"/>
-      <c r="AG31" s="8"/>
-      <c r="AH31" s="8"/>
-      <c r="AI31" s="8"/>
-      <c r="AJ31" s="8"/>
-      <c r="AK31" s="8"/>
-      <c r="AL31" s="8"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
     </row>
     <row r="32" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="Q32" s="8"/>
-      <c r="R32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="T32" s="8"/>
-      <c r="U32" s="8"/>
-      <c r="V32" s="8"/>
-      <c r="W32" s="8"/>
-      <c r="X32" s="8"/>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="8"/>
-      <c r="AD32" s="8"/>
-      <c r="AE32" s="8"/>
-      <c r="AF32" s="8"/>
-      <c r="AG32" s="8"/>
-      <c r="AH32" s="8"/>
-      <c r="AI32" s="8"/>
-      <c r="AJ32" s="8"/>
-      <c r="AK32" s="8"/>
-      <c r="AL32" s="8"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
     </row>
     <row r="33" spans="2:38" x14ac:dyDescent="0.35">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="8"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="8"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="8"/>
-      <c r="AC33" s="8"/>
-      <c r="AD33" s="8"/>
-      <c r="AE33" s="8"/>
-      <c r="AF33" s="8"/>
-      <c r="AG33" s="8"/>
-      <c r="AH33" s="8"/>
-      <c r="AI33" s="8"/>
-      <c r="AJ33" s="8"/>
-      <c r="AK33" s="8"/>
-      <c r="AL33" s="8"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10884,7 +11306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB1CE43-FC53-4439-A77E-9307732A5DBC}">
   <dimension ref="B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -10905,8 +11327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B359B592-07C0-44E5-81F1-1E3ECF7FDCC6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10920,8 +11342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D41C7B9-AC72-4DF7-9D48-3124C87DBACD}">
   <dimension ref="B24:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>